<commit_message>
get startups finance data
</commit_message>
<xml_diff>
--- a/startups_sum.xlsx
+++ b/startups_sum.xlsx
@@ -266,9 +266,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>NONE</t>
-  </si>
-  <si>
     <t>未融资</t>
     <rPh sb="0" eb="1">
       <t>wei rong zi</t>
@@ -300,9 +297,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>PRE_A</t>
-  </si>
-  <si>
     <t>Pre-A轮</t>
     <rPh sb="5" eb="6">
       <t>lun</t>
@@ -310,9 +304,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>IPO</t>
-  </si>
-  <si>
     <t>上市</t>
     <rPh sb="0" eb="1">
       <t>shang shi</t>
@@ -342,9 +333,6 @@
   <si>
     <t>INFORMAL</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEED</t>
   </si>
   <si>
     <t>种子轮</t>
@@ -402,9 +390,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>UNKNOWN</t>
-  </si>
-  <si>
     <t>未知</t>
     <rPh sb="0" eb="1">
       <t>wei zhi</t>
@@ -634,6 +619,26 @@
   </si>
   <si>
     <t>ACQUIRED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UNKNOWN</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NONE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IPO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRE_A</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1121,7 +1126,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1153,13 +1158,13 @@
         <v>74</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="K1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
@@ -1173,22 +1178,22 @@
         <v>15032</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F2" s="4">
         <v>279</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J2" s="4">
         <v>4327</v>
       </c>
       <c r="K2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1202,22 +1207,22 @@
         <v>922</v>
       </c>
       <c r="E3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F3" s="4">
         <v>5717</v>
       </c>
       <c r="G3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J3" s="4">
         <v>7723</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
@@ -1231,22 +1236,22 @@
         <v>387</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F4" s="4">
         <v>75</v>
       </c>
       <c r="G4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I4" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="J4" s="4">
         <v>1232</v>
       </c>
       <c r="K4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
@@ -1260,22 +1265,22 @@
         <v>216</v>
       </c>
       <c r="E5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F5" s="4">
         <v>1633</v>
       </c>
       <c r="G5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I5" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="J5" s="4">
         <v>257</v>
       </c>
       <c r="K5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
@@ -1289,22 +1294,22 @@
         <v>114</v>
       </c>
       <c r="E6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6" s="4">
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="J6" s="4">
         <v>2364</v>
       </c>
       <c r="K6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
@@ -1318,22 +1323,22 @@
         <v>743</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F7" s="4">
         <v>482</v>
       </c>
       <c r="G7" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="J7" s="4">
         <v>2418</v>
       </c>
       <c r="K7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
@@ -1347,22 +1352,22 @@
         <v>207</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F8" s="4">
         <v>232</v>
       </c>
       <c r="G8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J8" s="4">
         <v>184</v>
       </c>
       <c r="K8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
@@ -1376,22 +1381,22 @@
         <v>229</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F9" s="4">
         <v>106</v>
       </c>
       <c r="G9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="I9" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="J9" s="4">
         <v>2905</v>
       </c>
       <c r="K9" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
@@ -1405,22 +1410,22 @@
         <v>9750</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I10" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J10" s="4">
         <v>13243</v>
       </c>
       <c r="K10" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
@@ -1434,22 +1439,22 @@
         <v>3621</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>153</v>
       </c>
       <c r="F11" s="4">
         <v>1503</v>
       </c>
       <c r="G11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="J11" s="4">
         <v>5185</v>
       </c>
       <c r="K11" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
@@ -1463,22 +1468,22 @@
         <v>5111</v>
       </c>
       <c r="E12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F12" s="4">
         <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I12" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J12" s="4">
         <v>6582</v>
       </c>
       <c r="K12" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
@@ -1492,22 +1497,22 @@
         <v>702</v>
       </c>
       <c r="E13" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F13" s="4">
         <v>1099</v>
       </c>
       <c r="G13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I13" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="J13" s="4">
         <v>4771</v>
       </c>
       <c r="K13" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
@@ -1521,22 +1526,22 @@
         <v>1970</v>
       </c>
       <c r="E14" t="s">
-        <v>84</v>
+        <v>152</v>
       </c>
       <c r="F14" s="4">
         <v>1200</v>
       </c>
       <c r="G14" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I14" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="J14" s="4">
         <v>3221</v>
       </c>
       <c r="K14" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.15">
@@ -1550,22 +1555,22 @@
         <v>440</v>
       </c>
       <c r="E15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F15" s="4">
         <v>10405</v>
       </c>
       <c r="G15" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I15" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="J15" s="4">
         <v>736</v>
       </c>
       <c r="K15" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
@@ -1579,22 +1584,22 @@
         <v>1469</v>
       </c>
       <c r="E16" t="s">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="F16" s="4">
         <v>41776</v>
       </c>
       <c r="G16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I16" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="J16" s="4">
         <v>354</v>
       </c>
       <c r="K16" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
@@ -1608,22 +1613,22 @@
         <v>890</v>
       </c>
       <c r="E17" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="F17" s="4">
         <v>487</v>
       </c>
       <c r="G17" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="I17" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J17" s="4">
         <v>348</v>
       </c>
       <c r="K17" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.15">
@@ -1637,22 +1642,22 @@
         <v>1542</v>
       </c>
       <c r="E18" t="s">
-        <v>92</v>
+        <v>151</v>
       </c>
       <c r="F18" s="4">
         <v>374</v>
       </c>
       <c r="G18" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I18" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="J18" s="4">
         <v>868</v>
       </c>
       <c r="K18" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.15">
@@ -1666,13 +1671,13 @@
         <v>961</v>
       </c>
       <c r="I19" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="J19" s="4">
         <v>331</v>
       </c>
       <c r="K19" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
@@ -1686,13 +1691,13 @@
         <v>12818</v>
       </c>
       <c r="I20" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="J20" s="4">
         <v>1777</v>
       </c>
       <c r="K20" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
@@ -1706,13 +1711,13 @@
         <v>296</v>
       </c>
       <c r="I21" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="J21" s="4">
         <v>2865</v>
       </c>
       <c r="K21" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.15">
@@ -1726,13 +1731,13 @@
         <v>164</v>
       </c>
       <c r="I22" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="J22" s="4">
         <v>3697</v>
       </c>
       <c r="K22" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.15">

</xml_diff>